<commit_message>
sucsesfully refactord from service(The name of the old pakege) to 'Favor' the new name of the 'Service' class
</commit_message>
<xml_diff>
--- a/Documents/ПримерниДанни.xlsx
+++ b/Documents/ПримерниДанни.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivail\_Spring\GitLocalBackup\TicketSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A74BF315-1F7D-45BB-AE77-D69AE8B178FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847D10F-23A2-4732-A412-DD355273E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BDBF2F6-7486-411C-892F-AE32BE4E4AFF}"/>
   </bookViews>
@@ -1191,8 +1191,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623AB37B-1123-4DDE-8152-8795E823DD52}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I47" sqref="I47"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Started work on transactional and pakage naming
</commit_message>
<xml_diff>
--- a/Documents/ПримерниДанни.xlsx
+++ b/Documents/ПримерниДанни.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivail\_Spring\GitLocalBackup\TicketSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B847D10F-23A2-4732-A412-DD355273E05D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311898C-A3DE-4202-81C3-D9C3E5D35A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BDBF2F6-7486-411C-892F-AE32BE4E4AFF}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7BDBF2F6-7486-411C-892F-AE32BE4E4AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -704,18 +704,12 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -742,32 +736,49 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -849,6 +860,104 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF94545"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8686B"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1191,8 +1300,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623AB37B-1123-4DDE-8152-8795E823DD52}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1235,17 +1344,17 @@
       <c r="A3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="30" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="30"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="1" t="s">
@@ -1265,10 +1374,10 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>35</v>
       </c>
       <c r="D5" s="3" t="s">
@@ -1285,7 +1394,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="4">
@@ -1305,7 +1414,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="11" t="s">
         <v>14</v>
       </c>
       <c r="C7" s="4">
@@ -1325,7 +1434,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1345,119 +1454,119 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="19" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="E12" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="F12" s="21" t="s">
+      <c r="F12" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="13" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15"/>
-      <c r="F13" s="15"/>
-      <c r="G13" s="15"/>
+      <c r="C13" s="31"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="1" t="s">
         <v>57</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="1" t="s">
         <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="1" t="s">
         <v>58</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="1" t="s">
         <v>89</v>
       </c>
       <c r="G15" s="3" t="s">
@@ -1465,7 +1574,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="14" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="4">
@@ -1485,7 +1594,7 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="14" t="s">
         <v>14</v>
       </c>
       <c r="C17" s="4">
@@ -1505,7 +1614,7 @@
       </c>
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="14" t="s">
         <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
@@ -1525,7 +1634,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="14" t="s">
         <v>90</v>
       </c>
       <c r="C19" s="1" t="s">
@@ -1545,17 +1654,17 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="23" t="s">
+      <c r="B20" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="23"/>
-      <c r="D20" s="23"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="23"/>
-      <c r="G20" s="23"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="21"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B21" s="17" t="s">
+      <c r="B21" s="15" t="s">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
@@ -1575,7 +1684,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B22" s="17" t="s">
+      <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
       <c r="C22" s="1" t="s">
@@ -1595,7 +1704,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B23" s="17" t="s">
+      <c r="B23" s="15" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="2">
@@ -1615,7 +1724,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B24" s="17" t="s">
+      <c r="B24" s="15" t="s">
         <v>18</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1635,17 +1744,17 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="22"/>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="22"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="E25" s="20"/>
+      <c r="F25" s="20"/>
+      <c r="G25" s="20"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C26" s="1" t="s">
@@ -1665,19 +1774,19 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="14" t="s">
+      <c r="C27" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="E27" s="21" t="s">
+      <c r="E27" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="F27" s="14" t="s">
+      <c r="F27" s="13" t="s">
         <v>58</v>
       </c>
       <c r="G27" s="3" t="s">
@@ -1685,7 +1794,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B28" s="18" t="s">
+      <c r="B28" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C28" s="4">
@@ -1705,7 +1814,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B29" s="18" t="s">
+      <c r="B29" s="16" t="s">
         <v>14</v>
       </c>
       <c r="C29" s="4">
@@ -1725,7 +1834,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B30" s="18" t="s">
+      <c r="B30" s="16" t="s">
         <v>20</v>
       </c>
       <c r="C30" s="5" t="s">
@@ -1745,7 +1854,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B31" s="18" t="s">
+      <c r="B31" s="16" t="s">
         <v>21</v>
       </c>
       <c r="C31" s="5">
@@ -1765,7 +1874,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="16" t="s">
         <v>16</v>
       </c>
       <c r="C32" s="1" t="s">
@@ -1785,17 +1894,17 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="22"/>
-      <c r="D33" s="22"/>
-      <c r="E33" s="22"/>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
+      <c r="G33" s="34"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B34" s="18" t="s">
+      <c r="B34" s="16" t="s">
         <v>12</v>
       </c>
       <c r="C34" s="1" t="s">
@@ -1815,19 +1924,19 @@
       </c>
     </row>
     <row r="35" spans="2:7" ht="72.5" x14ac:dyDescent="0.35">
-      <c r="B35" s="19" t="s">
+      <c r="B35" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="F35" s="21" t="s">
+      <c r="F35" s="19" t="s">
         <v>100</v>
       </c>
       <c r="G35" s="3" t="s">
@@ -1835,7 +1944,7 @@
       </c>
     </row>
     <row r="36" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="16" t="s">
         <v>22</v>
       </c>
       <c r="C36" s="5" t="s">
@@ -1855,7 +1964,7 @@
       </c>
     </row>
     <row r="37" spans="2:7" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B37" s="18" t="s">
+      <c r="B37" s="16" t="s">
         <v>23</v>
       </c>
       <c r="C37" s="5" t="s">
@@ -1875,7 +1984,7 @@
       </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B38" s="18" t="s">
+      <c r="B38" s="16" t="s">
         <v>24</v>
       </c>
       <c r="C38" s="5" t="s">
@@ -1895,7 +2004,7 @@
       </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B39" s="18" t="s">
+      <c r="B39" s="16" t="s">
         <v>25</v>
       </c>
       <c r="C39" s="5" t="s">
@@ -1915,7 +2024,7 @@
       </c>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B40" s="18" t="s">
+      <c r="B40" s="16" t="s">
         <v>99</v>
       </c>
       <c r="C40" s="5" t="s">
@@ -1935,17 +2044,17 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="24" t="s">
+      <c r="B41" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="25"/>
-      <c r="D41" s="25"/>
-      <c r="E41" s="25"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="26"/>
+      <c r="C41" s="23"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="23"/>
+      <c r="F41" s="23"/>
+      <c r="G41" s="24"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B42" s="18" t="s">
+      <c r="B42" s="16" t="s">
         <v>17</v>
       </c>
       <c r="C42" s="2">
@@ -1965,7 +2074,7 @@
       </c>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" s="18" t="s">
+      <c r="B43" s="16" t="s">
         <v>26</v>
       </c>
       <c r="C43" s="4">
@@ -1985,7 +2094,7 @@
       </c>
     </row>
     <row r="44" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B44" s="18" t="s">
+      <c r="B44" s="16" t="s">
         <v>27</v>
       </c>
       <c r="C44" s="5" t="s">
@@ -2005,17 +2114,17 @@
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" s="27" t="s">
+      <c r="B45" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="27"/>
-      <c r="D45" s="27"/>
-      <c r="E45" s="27"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="27"/>
+      <c r="C45" s="36"/>
+      <c r="D45" s="36"/>
+      <c r="E45" s="36"/>
+      <c r="F45" s="36"/>
+      <c r="G45" s="37"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="18" t="s">
         <v>28</v>
       </c>
       <c r="C46" s="1" t="s">
@@ -2035,7 +2144,7 @@
       </c>
     </row>
     <row r="47" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="18" t="s">
         <v>29</v>
       </c>
       <c r="C47" s="1" t="s">
@@ -2055,7 +2164,7 @@
       </c>
     </row>
     <row r="48" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B48" s="20" t="s">
+      <c r="B48" s="18" t="s">
         <v>30</v>
       </c>
       <c r="C48" s="6" t="s">
@@ -2075,7 +2184,7 @@
       </c>
     </row>
     <row r="49" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="18" t="s">
         <v>31</v>
       </c>
       <c r="C49" s="7" t="s">
@@ -2090,12 +2199,12 @@
       <c r="F49" s="5">
         <v>12345679</v>
       </c>
-      <c r="G49" s="34">
+      <c r="G49" s="28">
         <v>12345678</v>
       </c>
     </row>
     <row r="50" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B50" s="20" t="s">
+      <c r="B50" s="18" t="s">
         <v>32</v>
       </c>
       <c r="C50" s="1" t="s">
@@ -2115,7 +2224,7 @@
       </c>
     </row>
     <row r="51" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B51" s="20" t="s">
+      <c r="B51" s="18" t="s">
         <v>18</v>
       </c>
       <c r="C51" s="1" t="s">
@@ -2135,7 +2244,7 @@
       </c>
     </row>
     <row r="52" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B52" s="20" t="s">
+      <c r="B52" s="18" t="s">
         <v>33</v>
       </c>
       <c r="C52" s="5">
@@ -2155,17 +2264,17 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="28" t="s">
+      <c r="B53" s="29" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="28"/>
-      <c r="D53" s="28"/>
-      <c r="E53" s="28"/>
-      <c r="F53" s="28"/>
-      <c r="G53" s="28"/>
+      <c r="C53" s="29"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="29"/>
+      <c r="G53" s="29"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="29" t="s">
+      <c r="B54" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2185,19 +2294,19 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B55" s="29" t="s">
+      <c r="B55" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="31" t="s">
+      <c r="C55" s="26" t="s">
         <v>132</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="D55" s="13" t="s">
         <v>136</v>
       </c>
-      <c r="E55" s="14" t="s">
+      <c r="E55" s="13" t="s">
         <v>139</v>
       </c>
-      <c r="F55" s="21" t="s">
+      <c r="F55" s="19" t="s">
         <v>142</v>
       </c>
       <c r="G55" s="1" t="s">
@@ -2205,7 +2314,7 @@
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="29" t="s">
+      <c r="B56" s="25" t="s">
         <v>130</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2225,7 +2334,7 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B57" s="29" t="s">
+      <c r="B57" s="25" t="s">
         <v>131</v>
       </c>
       <c r="C57" s="5">
@@ -2245,89 +2354,91 @@
       </c>
     </row>
     <row r="58" spans="2:7" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="32" t="s">
+      <c r="B58" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C58" s="33" t="s">
+      <c r="C58" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="D58" s="21" t="s">
+      <c r="D58" s="19" t="s">
         <v>135</v>
       </c>
-      <c r="E58" s="21" t="s">
+      <c r="E58" s="19" t="s">
         <v>138</v>
       </c>
-      <c r="F58" s="33" t="s">
+      <c r="F58" s="19" t="s">
         <v>143</v>
       </c>
-      <c r="G58" s="21" t="s">
+      <c r="G58" s="19" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="59" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B33:G33"/>
+    <mergeCell ref="B45:G45"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="13" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="58" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="12" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="57" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:F40 C30:G30 C44:G44">
-    <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="59" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="60" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
More work traing to make the jwt to work
</commit_message>
<xml_diff>
--- a/Documents/ПримерниДанни.xlsx
+++ b/Documents/ПримерниДанни.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivail\_Spring\GitLocalBackup\TicketSystem\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ivail\_Spring\ZipDanloads\TicketSystem\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7311898C-A3DE-4202-81C3-D9C3E5D35A36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38FED0D8-3CBB-4F24-833E-6152E970B249}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7BDBF2F6-7486-411C-892F-AE32BE4E4AFF}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7BDBF2F6-7486-411C-892F-AE32BE4E4AFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -680,7 +680,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -721,21 +721,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -771,6 +756,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -778,7 +772,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="14">
     <dxf>
       <fill>
         <patternFill>
@@ -860,104 +854,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF94545"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF8686B"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1300,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623AB37B-1123-4DDE-8152-8795E823DD52}">
   <dimension ref="A1:G59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A45" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45:G45"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1344,14 +1240,14 @@
       <c r="A3" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-      <c r="E3" s="30"/>
-      <c r="F3" s="30"/>
-      <c r="G3" s="30"/>
+      <c r="C3" s="25"/>
+      <c r="D3" s="25"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B4" s="11" t="s">
@@ -1454,14 +1350,14 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
@@ -1524,14 +1420,14 @@
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B13" s="31" t="s">
+      <c r="B13" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="31"/>
-      <c r="F13" s="31"/>
-      <c r="G13" s="31"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
+      <c r="E13" s="26"/>
+      <c r="F13" s="26"/>
+      <c r="G13" s="26"/>
     </row>
     <row r="14" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="14" t="s">
@@ -1654,14 +1550,14 @@
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B20" s="21" t="s">
+      <c r="B20" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="34"/>
+      <c r="E20" s="34"/>
+      <c r="F20" s="34"/>
+      <c r="G20" s="35"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B21" s="15" t="s">
@@ -1744,14 +1640,14 @@
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B25" s="20" t="s">
+      <c r="B25" s="27" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="20"/>
-      <c r="E25" s="20"/>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="29"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B26" s="16" t="s">
@@ -1894,14 +1790,14 @@
       </c>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B33" s="32" t="s">
+      <c r="B33" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C33" s="33"/>
-      <c r="D33" s="33"/>
-      <c r="E33" s="33"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="28"/>
+      <c r="E33" s="28"/>
+      <c r="F33" s="28"/>
+      <c r="G33" s="29"/>
     </row>
     <row r="34" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B34" s="16" t="s">
@@ -2044,14 +1940,14 @@
       </c>
     </row>
     <row r="41" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C41" s="23"/>
-      <c r="D41" s="23"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="23"/>
-      <c r="G41" s="24"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="28"/>
+      <c r="F41" s="28"/>
+      <c r="G41" s="29"/>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B42" s="16" t="s">
@@ -2114,14 +2010,14 @@
       </c>
     </row>
     <row r="45" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B45" s="35" t="s">
+      <c r="B45" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="C45" s="36"/>
-      <c r="D45" s="36"/>
-      <c r="E45" s="36"/>
-      <c r="F45" s="36"/>
-      <c r="G45" s="37"/>
+      <c r="C45" s="31"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="31"/>
+      <c r="G45" s="32"/>
     </row>
     <row r="46" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B46" s="18" t="s">
@@ -2199,7 +2095,7 @@
       <c r="F49" s="5">
         <v>12345679</v>
       </c>
-      <c r="G49" s="28">
+      <c r="G49" s="23">
         <v>12345678</v>
       </c>
     </row>
@@ -2264,17 +2160,17 @@
       </c>
     </row>
     <row r="53" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B53" s="29" t="s">
+      <c r="B53" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="C53" s="29"/>
-      <c r="D53" s="29"/>
-      <c r="E53" s="29"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
+      <c r="F53" s="24"/>
+      <c r="G53" s="24"/>
     </row>
     <row r="54" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B54" s="25" t="s">
+      <c r="B54" s="20" t="s">
         <v>16</v>
       </c>
       <c r="C54" s="1" t="s">
@@ -2294,10 +2190,10 @@
       </c>
     </row>
     <row r="55" spans="2:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="20" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="26" t="s">
+      <c r="C55" s="21" t="s">
         <v>132</v>
       </c>
       <c r="D55" s="13" t="s">
@@ -2309,12 +2205,12 @@
       <c r="F55" s="19" t="s">
         <v>142</v>
       </c>
-      <c r="G55" s="1" t="s">
+      <c r="G55" s="13" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="56" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B56" s="25" t="s">
+      <c r="B56" s="20" t="s">
         <v>130</v>
       </c>
       <c r="C56" s="1" t="s">
@@ -2334,7 +2230,7 @@
       </c>
     </row>
     <row r="57" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B57" s="25" t="s">
+      <c r="B57" s="20" t="s">
         <v>131</v>
       </c>
       <c r="C57" s="5">
@@ -2343,7 +2239,7 @@
       <c r="D57" s="5">
         <v>540578</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E57" s="2">
         <v>100123</v>
       </c>
       <c r="F57" s="2">
@@ -2354,7 +2250,7 @@
       </c>
     </row>
     <row r="58" spans="2:7" ht="84" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="22" t="s">
         <v>137</v>
       </c>
       <c r="C58" s="19" t="s">
@@ -2375,70 +2271,73 @@
     </row>
     <row r="59" spans="2:7" ht="30.5" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="9">
     <mergeCell ref="B53:G53"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B9:G9"/>
     <mergeCell ref="B13:G13"/>
     <mergeCell ref="B33:G33"/>
     <mergeCell ref="B45:G45"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B25:G25"/>
+    <mergeCell ref="B41:G41"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <conditionalFormatting sqref="A3">
-    <cfRule type="cellIs" dxfId="27" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="58" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="cellIs" dxfId="26" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="57" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:F40 C30:G30 C44:G44">
-    <cfRule type="cellIs" dxfId="14" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="59" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="60" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G36">
-    <cfRule type="cellIs" dxfId="24" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="9" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G38">
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G39">
-    <cfRule type="cellIs" dxfId="16" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>$A$3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>$A$2</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>